<commit_message>
xong sao luu + khoi phuc
</commit_message>
<xml_diff>
--- a/database/seeders/_nhan_vien_va_giao_vien_seeder.xlsx
+++ b/database/seeders/_nhan_vien_va_giao_vien_seeder.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8196" firstSheet="4" activeTab="8"/>
+    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8190" firstSheet="4" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="roles" sheetId="6" r:id="rId1"/>
@@ -1300,7 +1300,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1671,13 +1671,13 @@
       <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.33203125" customWidth="1"/>
-    <col min="2" max="2" width="31.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.28515625" customWidth="1"/>
+    <col min="2" max="2" width="31.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>8</v>
       </c>
@@ -1685,7 +1685,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>59</v>
       </c>
@@ -1693,7 +1693,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>57</v>
       </c>
@@ -1701,7 +1701,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>55</v>
       </c>
@@ -1709,7 +1709,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>53</v>
       </c>
@@ -1730,9 +1730,9 @@
       <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>325</v>
       </c>
@@ -1749,7 +1749,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>330</v>
       </c>
@@ -1763,7 +1763,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>330</v>
       </c>
@@ -1777,7 +1777,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>330</v>
       </c>
@@ -1791,7 +1791,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>332</v>
       </c>
@@ -1805,7 +1805,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>332</v>
       </c>
@@ -1819,7 +1819,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>332</v>
       </c>
@@ -1833,7 +1833,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>330</v>
       </c>
@@ -1847,7 +1847,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>330</v>
       </c>
@@ -1861,7 +1861,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>330</v>
       </c>
@@ -1875,7 +1875,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>332</v>
       </c>
@@ -1889,7 +1889,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>332</v>
       </c>
@@ -1903,7 +1903,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>332</v>
       </c>
@@ -1930,13 +1930,13 @@
       <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="38.44140625" customWidth="1"/>
-    <col min="2" max="2" width="21.44140625" customWidth="1"/>
+    <col min="1" max="1" width="38.42578125" customWidth="1"/>
+    <col min="2" max="2" width="21.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>249</v>
       </c>
@@ -1944,7 +1944,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>247</v>
       </c>
@@ -1952,7 +1952,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>246</v>
       </c>
@@ -1960,7 +1960,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>245</v>
       </c>
@@ -1968,7 +1968,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>244</v>
       </c>
@@ -1976,7 +1976,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>243</v>
       </c>
@@ -1984,7 +1984,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>242</v>
       </c>
@@ -1992,7 +1992,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>241</v>
       </c>
@@ -2000,7 +2000,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>240</v>
       </c>
@@ -2008,7 +2008,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>239</v>
       </c>
@@ -2016,7 +2016,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>238</v>
       </c>
@@ -2024,7 +2024,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>237</v>
       </c>
@@ -2032,7 +2032,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>236</v>
       </c>
@@ -2040,7 +2040,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>235</v>
       </c>
@@ -2048,7 +2048,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>234</v>
       </c>
@@ -2056,7 +2056,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>233</v>
       </c>
@@ -2064,7 +2064,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>232</v>
       </c>
@@ -2072,7 +2072,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>231</v>
       </c>
@@ -2080,7 +2080,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>230</v>
       </c>
@@ -2088,7 +2088,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>229</v>
       </c>
@@ -2096,7 +2096,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>228</v>
       </c>
@@ -2104,7 +2104,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>227</v>
       </c>
@@ -2126,14 +2126,14 @@
       <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="27.109375" customWidth="1"/>
-    <col min="2" max="2" width="32.33203125" customWidth="1"/>
-    <col min="3" max="3" width="21.6640625" customWidth="1"/>
+    <col min="1" max="1" width="27.140625" customWidth="1"/>
+    <col min="2" max="2" width="32.28515625" customWidth="1"/>
+    <col min="3" max="3" width="21.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>8</v>
       </c>
@@ -2144,7 +2144,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>225</v>
       </c>
@@ -2155,7 +2155,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>223</v>
       </c>
@@ -2166,7 +2166,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>221</v>
       </c>
@@ -2177,7 +2177,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>219</v>
       </c>
@@ -2188,7 +2188,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>217</v>
       </c>
@@ -2199,7 +2199,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>215</v>
       </c>
@@ -2210,7 +2210,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>213</v>
       </c>
@@ -2221,7 +2221,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>211</v>
       </c>
@@ -2232,7 +2232,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>209</v>
       </c>
@@ -2243,7 +2243,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>207</v>
       </c>
@@ -2254,7 +2254,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>205</v>
       </c>
@@ -2265,7 +2265,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>203</v>
       </c>
@@ -2276,7 +2276,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>201</v>
       </c>
@@ -2287,7 +2287,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>199</v>
       </c>
@@ -2298,7 +2298,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>197</v>
       </c>
@@ -2309,7 +2309,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>195</v>
       </c>
@@ -2320,7 +2320,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>193</v>
       </c>
@@ -2331,7 +2331,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>191</v>
       </c>
@@ -2342,7 +2342,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>189</v>
       </c>
@@ -2353,7 +2353,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>187</v>
       </c>
@@ -2364,7 +2364,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>185</v>
       </c>
@@ -2375,7 +2375,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>183</v>
       </c>
@@ -2386,7 +2386,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>181</v>
       </c>
@@ -2397,7 +2397,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>179</v>
       </c>
@@ -2408,7 +2408,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>177</v>
       </c>
@@ -2419,7 +2419,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>175</v>
       </c>
@@ -2430,7 +2430,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>173</v>
       </c>
@@ -2441,7 +2441,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>171</v>
       </c>
@@ -2452,7 +2452,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>169</v>
       </c>
@@ -2463,7 +2463,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>167</v>
       </c>
@@ -2474,7 +2474,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>165</v>
       </c>
@@ -2485,7 +2485,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>163</v>
       </c>
@@ -2496,7 +2496,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>161</v>
       </c>
@@ -2507,7 +2507,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>159</v>
       </c>
@@ -2518,7 +2518,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>157</v>
       </c>
@@ -2529,7 +2529,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>155</v>
       </c>
@@ -2540,7 +2540,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>153</v>
       </c>
@@ -2551,7 +2551,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>151</v>
       </c>
@@ -2562,7 +2562,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>149</v>
       </c>
@@ -2573,7 +2573,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>147</v>
       </c>
@@ -2584,7 +2584,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>145</v>
       </c>
@@ -2595,7 +2595,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>143</v>
       </c>
@@ -2606,7 +2606,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>141</v>
       </c>
@@ -2617,7 +2617,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>139</v>
       </c>
@@ -2628,7 +2628,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>137</v>
       </c>
@@ -2639,7 +2639,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>135</v>
       </c>
@@ -2650,7 +2650,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>133</v>
       </c>
@@ -2661,7 +2661,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>131</v>
       </c>
@@ -2672,7 +2672,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>129</v>
       </c>
@@ -2683,7 +2683,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>127</v>
       </c>
@@ -2694,7 +2694,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>125</v>
       </c>
@@ -2705,7 +2705,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>123</v>
       </c>
@@ -2716,7 +2716,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>121</v>
       </c>
@@ -2727,7 +2727,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>119</v>
       </c>
@@ -2738,7 +2738,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>117</v>
       </c>
@@ -2749,7 +2749,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>115</v>
       </c>
@@ -2760,7 +2760,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>113</v>
       </c>
@@ -2771,7 +2771,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>111</v>
       </c>
@@ -2782,7 +2782,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>109</v>
       </c>
@@ -2793,7 +2793,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>107</v>
       </c>
@@ -2804,7 +2804,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>105</v>
       </c>
@@ -2815,7 +2815,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>103</v>
       </c>
@@ -2826,7 +2826,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>101</v>
       </c>
@@ -2837,7 +2837,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>99</v>
       </c>
@@ -2848,7 +2848,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>97</v>
       </c>
@@ -2859,7 +2859,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>95</v>
       </c>
@@ -2870,7 +2870,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>93</v>
       </c>
@@ -2881,7 +2881,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>91</v>
       </c>
@@ -2892,7 +2892,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>89</v>
       </c>
@@ -2903,7 +2903,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>87</v>
       </c>
@@ -2914,7 +2914,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>85</v>
       </c>
@@ -2925,7 +2925,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>83</v>
       </c>
@@ -2936,7 +2936,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>81</v>
       </c>
@@ -2947,7 +2947,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>79</v>
       </c>
@@ -2958,7 +2958,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>77</v>
       </c>
@@ -2969,7 +2969,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>75</v>
       </c>
@@ -2980,7 +2980,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>73</v>
       </c>
@@ -2991,7 +2991,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>71</v>
       </c>
@@ -3002,7 +3002,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>69</v>
       </c>
@@ -3013,7 +3013,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>67</v>
       </c>
@@ -3024,7 +3024,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>65</v>
       </c>
@@ -3035,7 +3035,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>63</v>
       </c>
@@ -3046,7 +3046,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>61</v>
       </c>
@@ -3071,13 +3071,13 @@
       <selection activeCell="B196" sqref="B196"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="32.6640625" customWidth="1"/>
-    <col min="2" max="2" width="25.109375" customWidth="1"/>
+    <col min="1" max="1" width="32.7109375" customWidth="1"/>
+    <col min="2" max="2" width="25.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>251</v>
       </c>
@@ -3085,7 +3085,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -3093,7 +3093,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
@@ -3101,7 +3101,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2</v>
       </c>
@@ -3109,7 +3109,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>3</v>
       </c>
@@ -3117,7 +3117,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>4</v>
       </c>
@@ -3125,7 +3125,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>5</v>
       </c>
@@ -3133,7 +3133,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>5</v>
       </c>
@@ -3141,7 +3141,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>5</v>
       </c>
@@ -3149,7 +3149,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>5</v>
       </c>
@@ -3157,7 +3157,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>6</v>
       </c>
@@ -3165,7 +3165,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>6</v>
       </c>
@@ -3173,7 +3173,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>7</v>
       </c>
@@ -3181,7 +3181,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>7</v>
       </c>
@@ -3189,7 +3189,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>8</v>
       </c>
@@ -3197,7 +3197,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>8</v>
       </c>
@@ -3205,7 +3205,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>9</v>
       </c>
@@ -3213,7 +3213,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>9</v>
       </c>
@@ -3221,7 +3221,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>10</v>
       </c>
@@ -3229,7 +3229,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>10</v>
       </c>
@@ -3237,7 +3237,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>10</v>
       </c>
@@ -3245,7 +3245,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>10</v>
       </c>
@@ -3253,7 +3253,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>11</v>
       </c>
@@ -3261,7 +3261,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>11</v>
       </c>
@@ -3269,7 +3269,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>12</v>
       </c>
@@ -3277,7 +3277,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>12</v>
       </c>
@@ -3285,7 +3285,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>13</v>
       </c>
@@ -3293,7 +3293,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>13</v>
       </c>
@@ -3301,7 +3301,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>14</v>
       </c>
@@ -3309,7 +3309,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>14</v>
       </c>
@@ -3317,7 +3317,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>14</v>
       </c>
@@ -3325,7 +3325,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>14</v>
       </c>
@@ -3333,7 +3333,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>15</v>
       </c>
@@ -3341,7 +3341,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>15</v>
       </c>
@@ -3349,7 +3349,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>15</v>
       </c>
@@ -3357,7 +3357,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>16</v>
       </c>
@@ -3365,7 +3365,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>16</v>
       </c>
@@ -3373,7 +3373,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>16</v>
       </c>
@@ -3381,7 +3381,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>17</v>
       </c>
@@ -3389,7 +3389,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>17</v>
       </c>
@@ -3397,7 +3397,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>17</v>
       </c>
@@ -3405,7 +3405,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>18</v>
       </c>
@@ -3413,7 +3413,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>18</v>
       </c>
@@ -3421,7 +3421,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>18</v>
       </c>
@@ -3429,7 +3429,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>18</v>
       </c>
@@ -3437,7 +3437,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>19</v>
       </c>
@@ -3445,7 +3445,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>19</v>
       </c>
@@ -3453,7 +3453,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>19</v>
       </c>
@@ -3461,7 +3461,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>20</v>
       </c>
@@ -3469,7 +3469,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>20</v>
       </c>
@@ -3477,7 +3477,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>20</v>
       </c>
@@ -3485,7 +3485,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>21</v>
       </c>
@@ -3493,7 +3493,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>21</v>
       </c>
@@ -3501,7 +3501,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>21</v>
       </c>
@@ -3509,7 +3509,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>22</v>
       </c>
@@ -3517,7 +3517,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>22</v>
       </c>
@@ -3525,7 +3525,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>22</v>
       </c>
@@ -3533,7 +3533,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>22</v>
       </c>
@@ -3541,7 +3541,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>23</v>
       </c>
@@ -3549,7 +3549,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>23</v>
       </c>
@@ -3557,7 +3557,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>24</v>
       </c>
@@ -3565,7 +3565,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>24</v>
       </c>
@@ -3573,7 +3573,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>25</v>
       </c>
@@ -3581,7 +3581,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>25</v>
       </c>
@@ -3589,7 +3589,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>26</v>
       </c>
@@ -3597,7 +3597,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>26</v>
       </c>
@@ -3605,7 +3605,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>26</v>
       </c>
@@ -3613,7 +3613,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>26</v>
       </c>
@@ -3621,7 +3621,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>27</v>
       </c>
@@ -3629,7 +3629,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>27</v>
       </c>
@@ -3637,7 +3637,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>28</v>
       </c>
@@ -3645,7 +3645,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>28</v>
       </c>
@@ -3653,7 +3653,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>29</v>
       </c>
@@ -3661,7 +3661,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>29</v>
       </c>
@@ -3669,7 +3669,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>30</v>
       </c>
@@ -3677,7 +3677,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>31</v>
       </c>
@@ -3685,7 +3685,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>31</v>
       </c>
@@ -3693,7 +3693,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>31</v>
       </c>
@@ -3701,7 +3701,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>31</v>
       </c>
@@ -3709,7 +3709,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>32</v>
       </c>
@@ -3717,7 +3717,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>32</v>
       </c>
@@ -3725,7 +3725,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>33</v>
       </c>
@@ -3733,7 +3733,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>33</v>
       </c>
@@ -3741,7 +3741,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>34</v>
       </c>
@@ -3749,7 +3749,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>34</v>
       </c>
@@ -3757,7 +3757,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A86">
         <v>35</v>
       </c>
@@ -3765,7 +3765,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A87">
         <v>35</v>
       </c>
@@ -3773,7 +3773,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A88">
         <v>36</v>
       </c>
@@ -3781,7 +3781,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A89">
         <v>36</v>
       </c>
@@ -3789,7 +3789,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A90">
         <v>36</v>
       </c>
@@ -3797,7 +3797,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A91">
         <v>36</v>
       </c>
@@ -3805,7 +3805,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A92">
         <v>37</v>
       </c>
@@ -3813,7 +3813,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A93">
         <v>37</v>
       </c>
@@ -3821,7 +3821,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A94">
         <v>38</v>
       </c>
@@ -3829,7 +3829,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A95">
         <v>38</v>
       </c>
@@ -3837,7 +3837,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A96">
         <v>38</v>
       </c>
@@ -3845,7 +3845,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A97">
         <v>39</v>
       </c>
@@ -3853,7 +3853,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A98">
         <v>39</v>
       </c>
@@ -3861,7 +3861,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A99">
         <v>40</v>
       </c>
@@ -3869,7 +3869,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A100">
         <v>40</v>
       </c>
@@ -3877,7 +3877,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A101">
         <v>40</v>
       </c>
@@ -3885,7 +3885,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="102" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A102">
         <v>40</v>
       </c>
@@ -3893,7 +3893,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="103" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A103">
         <v>41</v>
       </c>
@@ -3901,7 +3901,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="104" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A104">
         <v>41</v>
       </c>
@@ -3909,7 +3909,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="105" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A105">
         <v>42</v>
       </c>
@@ -3917,7 +3917,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="106" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A106">
         <v>42</v>
       </c>
@@ -3925,7 +3925,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="107" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A107">
         <v>43</v>
       </c>
@@ -3933,7 +3933,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="108" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A108">
         <v>43</v>
       </c>
@@ -3941,7 +3941,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="109" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A109">
         <v>44</v>
       </c>
@@ -3949,7 +3949,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="110" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A110">
         <v>44</v>
       </c>
@@ -3957,7 +3957,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="111" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A111">
         <v>44</v>
       </c>
@@ -3965,7 +3965,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="112" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A112">
         <v>44</v>
       </c>
@@ -3973,7 +3973,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="113" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A113">
         <v>45</v>
       </c>
@@ -3981,7 +3981,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="114" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A114">
         <v>45</v>
       </c>
@@ -3989,7 +3989,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="115" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A115">
         <v>45</v>
       </c>
@@ -3997,7 +3997,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="116" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A116">
         <v>46</v>
       </c>
@@ -4005,7 +4005,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="117" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A117">
         <v>46</v>
       </c>
@@ -4013,7 +4013,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="118" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A118">
         <v>46</v>
       </c>
@@ -4021,7 +4021,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="119" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A119">
         <v>47</v>
       </c>
@@ -4029,7 +4029,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="120" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A120">
         <v>47</v>
       </c>
@@ -4037,7 +4037,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="121" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A121">
         <v>47</v>
       </c>
@@ -4045,7 +4045,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="122" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A122">
         <v>48</v>
       </c>
@@ -4053,7 +4053,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="123" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A123">
         <v>48</v>
       </c>
@@ -4061,7 +4061,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="124" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A124">
         <v>48</v>
       </c>
@@ -4069,7 +4069,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="125" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A125">
         <v>48</v>
       </c>
@@ -4077,7 +4077,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="126" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A126">
         <v>49</v>
       </c>
@@ -4085,7 +4085,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="127" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A127">
         <v>49</v>
       </c>
@@ -4093,7 +4093,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="128" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A128">
         <v>50</v>
       </c>
@@ -4101,7 +4101,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="129" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A129">
         <v>50</v>
       </c>
@@ -4109,7 +4109,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="130" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A130">
         <v>51</v>
       </c>
@@ -4117,7 +4117,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="131" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A131">
         <v>51</v>
       </c>
@@ -4125,7 +4125,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="132" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A132">
         <v>52</v>
       </c>
@@ -4133,7 +4133,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="133" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A133">
         <v>52</v>
       </c>
@@ -4141,7 +4141,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="134" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A134">
         <v>53</v>
       </c>
@@ -4149,7 +4149,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="135" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A135">
         <v>53</v>
       </c>
@@ -4157,7 +4157,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="136" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A136">
         <v>54</v>
       </c>
@@ -4165,7 +4165,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="137" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A137">
         <v>54</v>
       </c>
@@ -4173,7 +4173,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="138" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A138">
         <v>55</v>
       </c>
@@ -4181,7 +4181,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="139" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A139">
         <v>55</v>
       </c>
@@ -4189,7 +4189,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="140" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A140">
         <v>56</v>
       </c>
@@ -4197,7 +4197,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="141" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A141">
         <v>56</v>
       </c>
@@ -4205,7 +4205,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="142" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A142">
         <v>56</v>
       </c>
@@ -4213,7 +4213,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="143" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A143">
         <v>56</v>
       </c>
@@ -4221,7 +4221,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="144" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A144">
         <v>57</v>
       </c>
@@ -4229,7 +4229,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="145" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A145">
         <v>57</v>
       </c>
@@ -4237,7 +4237,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="146" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A146">
         <v>58</v>
       </c>
@@ -4245,7 +4245,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="147" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A147">
         <v>58</v>
       </c>
@@ -4253,7 +4253,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="148" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A148">
         <v>59</v>
       </c>
@@ -4261,7 +4261,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="149" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A149">
         <v>59</v>
       </c>
@@ -4269,7 +4269,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="150" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A150">
         <v>60</v>
       </c>
@@ -4277,7 +4277,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="151" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A151">
         <v>60</v>
       </c>
@@ -4285,7 +4285,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="152" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A152">
         <v>61</v>
       </c>
@@ -4293,7 +4293,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="153" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A153">
         <v>61</v>
       </c>
@@ -4301,7 +4301,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="154" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A154">
         <v>62</v>
       </c>
@@ -4309,7 +4309,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="155" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A155">
         <v>62</v>
       </c>
@@ -4317,7 +4317,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="156" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A156">
         <v>63</v>
       </c>
@@ -4325,7 +4325,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="157" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A157">
         <v>63</v>
       </c>
@@ -4333,7 +4333,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="158" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A158">
         <v>64</v>
       </c>
@@ -4341,7 +4341,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="159" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A159">
         <v>64</v>
       </c>
@@ -4349,7 +4349,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="160" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A160">
         <v>65</v>
       </c>
@@ -4357,7 +4357,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="161" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A161">
         <v>65</v>
       </c>
@@ -4365,7 +4365,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="162" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A162">
         <v>66</v>
       </c>
@@ -4373,7 +4373,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="163" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A163">
         <v>66</v>
       </c>
@@ -4381,7 +4381,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="164" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A164">
         <v>67</v>
       </c>
@@ -4389,7 +4389,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="165" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A165">
         <v>67</v>
       </c>
@@ -4397,7 +4397,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="166" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A166">
         <v>68</v>
       </c>
@@ -4405,7 +4405,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="167" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A167">
         <v>68</v>
       </c>
@@ -4413,7 +4413,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="168" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A168">
         <v>69</v>
       </c>
@@ -4421,7 +4421,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="169" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A169">
         <v>69</v>
       </c>
@@ -4429,7 +4429,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="170" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A170">
         <v>70</v>
       </c>
@@ -4437,7 +4437,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="171" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A171">
         <v>71</v>
       </c>
@@ -4445,7 +4445,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="172" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A172">
         <v>72</v>
       </c>
@@ -4453,7 +4453,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="173" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A173">
         <v>72</v>
       </c>
@@ -4461,7 +4461,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="174" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A174">
         <v>73</v>
       </c>
@@ -4469,7 +4469,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="175" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="175" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A175">
         <v>73</v>
       </c>
@@ -4477,7 +4477,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="176" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="176" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A176">
         <v>74</v>
       </c>
@@ -4485,7 +4485,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="177" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="177" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A177">
         <v>74</v>
       </c>
@@ -4493,7 +4493,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="178" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="178" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A178">
         <v>75</v>
       </c>
@@ -4501,7 +4501,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="179" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="179" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A179">
         <v>75</v>
       </c>
@@ -4509,7 +4509,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="180" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="180" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A180">
         <v>76</v>
       </c>
@@ -4517,7 +4517,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="181" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="181" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A181">
         <v>76</v>
       </c>
@@ -4525,7 +4525,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="182" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="182" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A182">
         <v>76</v>
       </c>
@@ -4533,7 +4533,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="183" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="183" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A183">
         <v>77</v>
       </c>
@@ -4541,7 +4541,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="184" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="184" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A184">
         <v>77</v>
       </c>
@@ -4549,7 +4549,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="185" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="185" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A185">
         <v>77</v>
       </c>
@@ -4557,7 +4557,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="186" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="186" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A186">
         <v>78</v>
       </c>
@@ -4565,7 +4565,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="187" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="187" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A187">
         <v>78</v>
       </c>
@@ -4573,7 +4573,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="188" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="188" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A188">
         <v>78</v>
       </c>
@@ -4581,7 +4581,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="189" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="189" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A189">
         <v>79</v>
       </c>
@@ -4589,7 +4589,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="190" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="190" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A190">
         <v>79</v>
       </c>
@@ -4597,7 +4597,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="191" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="191" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A191">
         <v>79</v>
       </c>
@@ -4605,7 +4605,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="192" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="192" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A192">
         <v>80</v>
       </c>
@@ -4613,7 +4613,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="193" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="193" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A193">
         <v>81</v>
       </c>
@@ -4621,7 +4621,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="194" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="194" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A194">
         <v>82</v>
       </c>
@@ -4629,7 +4629,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="195" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="195" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A195">
         <v>83</v>
       </c>
@@ -4637,7 +4637,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="196" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="196" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A196">
         <v>1</v>
       </c>
@@ -4655,20 +4655,20 @@
   <dimension ref="A1:E51"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="80.88671875" style="4" customWidth="1"/>
-    <col min="2" max="2" width="15.6640625" style="4" customWidth="1"/>
-    <col min="3" max="3" width="84.44140625" style="4" customWidth="1"/>
-    <col min="4" max="4" width="15.88671875" style="4" customWidth="1"/>
-    <col min="5" max="5" width="13.88671875" style="4" customWidth="1"/>
-    <col min="6" max="16384" width="9.109375" style="4"/>
+    <col min="1" max="1" width="80.85546875" style="4" customWidth="1"/>
+    <col min="2" max="2" width="15.7109375" style="4" customWidth="1"/>
+    <col min="3" max="3" width="84.42578125" style="4" customWidth="1"/>
+    <col min="4" max="4" width="15.85546875" style="4" customWidth="1"/>
+    <col min="5" max="5" width="13.85546875" style="4" customWidth="1"/>
+    <col min="6" max="16384" width="9.140625" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>323</v>
       </c>
@@ -4685,7 +4685,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>320</v>
       </c>
@@ -4702,7 +4702,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>317</v>
       </c>
@@ -4719,7 +4719,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>314</v>
       </c>
@@ -4736,7 +4736,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>311</v>
       </c>
@@ -4753,7 +4753,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>308</v>
       </c>
@@ -4770,7 +4770,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>306</v>
       </c>
@@ -4787,7 +4787,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>304</v>
       </c>
@@ -4804,7 +4804,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>302</v>
       </c>
@@ -4821,7 +4821,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
         <v>300</v>
       </c>
@@ -4838,7 +4838,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
         <v>298</v>
       </c>
@@ -4855,7 +4855,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
         <v>296</v>
       </c>
@@ -4872,7 +4872,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
         <v>294</v>
       </c>
@@ -4889,7 +4889,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
         <v>292</v>
       </c>
@@ -4906,7 +4906,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
         <v>290</v>
       </c>
@@ -4923,7 +4923,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
         <v>288</v>
       </c>
@@ -4940,7 +4940,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
         <v>286</v>
       </c>
@@ -4957,7 +4957,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
         <v>284</v>
       </c>
@@ -4974,7 +4974,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
         <v>282</v>
       </c>
@@ -4991,7 +4991,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
         <v>280</v>
       </c>
@@ -5008,7 +5008,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
         <v>278</v>
       </c>
@@ -5025,7 +5025,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
         <v>276</v>
       </c>
@@ -5042,7 +5042,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
         <v>274</v>
       </c>
@@ -5059,7 +5059,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
         <v>272</v>
       </c>
@@ -5076,7 +5076,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="5" t="s">
         <v>270</v>
       </c>
@@ -5093,7 +5093,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="5" t="s">
         <v>268</v>
       </c>
@@ -5110,7 +5110,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="5" t="s">
         <v>266</v>
       </c>
@@ -5127,7 +5127,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="5" t="s">
         <v>264</v>
       </c>
@@ -5144,7 +5144,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="5" t="s">
         <v>262</v>
       </c>
@@ -5161,7 +5161,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="5" t="s">
         <v>260</v>
       </c>
@@ -5178,7 +5178,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="6" t="s">
         <v>414</v>
       </c>
@@ -5195,7 +5195,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="6" t="s">
         <v>413</v>
       </c>
@@ -5212,7 +5212,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="6" t="s">
         <v>412</v>
       </c>
@@ -5229,7 +5229,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="6" t="s">
         <v>411</v>
       </c>
@@ -5246,7 +5246,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="6" t="s">
         <v>410</v>
       </c>
@@ -5263,7 +5263,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="6" t="s">
         <v>409</v>
       </c>
@@ -5280,7 +5280,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="6" t="s">
         <v>408</v>
       </c>
@@ -5297,7 +5297,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="6" t="s">
         <v>416</v>
       </c>
@@ -5314,7 +5314,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="6" t="s">
         <v>415</v>
       </c>
@@ -5331,7 +5331,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="6" t="s">
         <v>417</v>
       </c>
@@ -5348,7 +5348,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="6" t="s">
         <v>418</v>
       </c>
@@ -5365,7 +5365,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="6" t="s">
         <v>419</v>
       </c>
@@ -5382,7 +5382,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="6" t="s">
         <v>420</v>
       </c>
@@ -5399,7 +5399,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="6" t="s">
         <v>421</v>
       </c>
@@ -5416,7 +5416,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="6" t="s">
         <v>422</v>
       </c>
@@ -5433,7 +5433,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="6" t="s">
         <v>407</v>
       </c>
@@ -5450,7 +5450,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" s="6" t="s">
         <v>406</v>
       </c>
@@ -5467,7 +5467,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" s="6" t="s">
         <v>405</v>
       </c>
@@ -5484,7 +5484,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" s="6" t="s">
         <v>404</v>
       </c>
@@ -5501,7 +5501,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" s="6" t="s">
         <v>403</v>
       </c>
@@ -5518,7 +5518,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" s="6" t="s">
         <v>402</v>
       </c>
@@ -5574,15 +5574,15 @@
       <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="31.6640625" customWidth="1"/>
-    <col min="2" max="2" width="27.44140625" customWidth="1"/>
+    <col min="1" max="1" width="31.7109375" customWidth="1"/>
+    <col min="2" max="2" width="27.42578125" customWidth="1"/>
     <col min="3" max="3" width="20" customWidth="1"/>
     <col min="4" max="4" width="17" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>8</v>
       </c>
@@ -5596,7 +5596,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -5610,7 +5610,7 @@
         <v>2000000</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -5624,7 +5624,7 @@
         <v>5000000</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -5638,7 +5638,7 @@
         <v>3000000</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>1</v>
       </c>
@@ -5665,14 +5665,14 @@
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.6640625" customWidth="1"/>
-    <col min="2" max="2" width="58.44140625" customWidth="1"/>
-    <col min="3" max="3" width="50.44140625" customWidth="1"/>
+    <col min="1" max="1" width="23.7109375" customWidth="1"/>
+    <col min="2" max="2" width="58.42578125" customWidth="1"/>
+    <col min="3" max="3" width="50.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>14</v>
       </c>
@@ -5683,7 +5683,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -5694,7 +5694,7 @@
         <v>150000</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -5715,21 +5715,21 @@
   <dimension ref="A1:K6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.88671875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="11.85546875" style="1" customWidth="1"/>
     <col min="2" max="2" width="28" customWidth="1"/>
-    <col min="4" max="4" width="17.6640625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="11.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="31.109375" customWidth="1"/>
-    <col min="9" max="9" width="17.5546875" customWidth="1"/>
-    <col min="10" max="10" width="14.109375" customWidth="1"/>
+    <col min="4" max="4" width="17.7109375" style="1" customWidth="1"/>
+    <col min="6" max="6" width="11.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="31.140625" customWidth="1"/>
+    <col min="9" max="9" width="17.5703125" customWidth="1"/>
+    <col min="10" max="10" width="14.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>34</v>
       </c>
@@ -5764,7 +5764,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>50</v>
       </c>
@@ -5799,7 +5799,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>45</v>
       </c>
@@ -5834,7 +5834,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>39</v>
       </c>
@@ -5863,16 +5863,16 @@
         <v>15</v>
       </c>
       <c r="J4">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="K4">
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="G5" s="2"/>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="G6" s="2"/>
     </row>
   </sheetData>
@@ -5889,20 +5889,21 @@
   <dimension ref="A1:K21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="J25" sqref="J25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.6640625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="17.33203125" customWidth="1"/>
-    <col min="4" max="4" width="15.6640625" customWidth="1"/>
-    <col min="6" max="6" width="31.33203125" customWidth="1"/>
-    <col min="7" max="7" width="25.44140625" customWidth="1"/>
-    <col min="9" max="9" width="16.44140625" customWidth="1"/>
+    <col min="1" max="1" width="22.7109375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="17.28515625" customWidth="1"/>
+    <col min="4" max="4" width="15.7109375" customWidth="1"/>
+    <col min="6" max="6" width="31.28515625" customWidth="1"/>
+    <col min="7" max="7" width="25.42578125" customWidth="1"/>
+    <col min="9" max="9" width="16.42578125" customWidth="1"/>
+    <col min="11" max="11" width="15.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>34</v>
       </c>
@@ -5937,7 +5938,7 @@
         <v>401</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>25</v>
       </c>
@@ -5972,7 +5973,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>21</v>
       </c>
@@ -6007,7 +6008,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>383</v>
       </c>
@@ -6042,7 +6043,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>378</v>
       </c>
@@ -6077,7 +6078,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>372</v>
       </c>
@@ -6112,7 +6113,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>367</v>
       </c>
@@ -6147,7 +6148,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>364</v>
       </c>
@@ -6182,7 +6183,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>361</v>
       </c>
@@ -6217,7 +6218,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>359</v>
       </c>
@@ -6252,7 +6253,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>356</v>
       </c>
@@ -6287,7 +6288,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>353</v>
       </c>
@@ -6322,7 +6323,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>351</v>
       </c>
@@ -6357,7 +6358,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>348</v>
       </c>
@@ -6392,7 +6393,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>345</v>
       </c>
@@ -6427,7 +6428,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>342</v>
       </c>
@@ -6462,7 +6463,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>339</v>
       </c>
@@ -6497,7 +6498,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>336</v>
       </c>
@@ -6532,7 +6533,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="F21" s="1"/>
     </row>
   </sheetData>

</xml_diff>